<commit_message>
doc(linux): statistics for tcp connections
</commit_message>
<xml_diff>
--- a/ide/IDEA、PyCharm默认快捷键说明.xlsx
+++ b/ide/IDEA、PyCharm默认快捷键说明.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11940"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -752,12 +752,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -792,66 +792,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -876,18 +816,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -900,15 +840,47 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,7 +902,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -971,19 +971,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,157 +1145,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,6 +1162,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1191,39 +1224,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1267,152 +1267,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1444,57 +1444,60 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1768,9 +1771,9 @@
   <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -2634,10 +2637,10 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="11" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
doc(mysql): implements full join use alternative method
</commit_message>
<xml_diff>
--- a/ide/IDEA、PyCharm默认快捷键说明.xlsx
+++ b/ide/IDEA、PyCharm默认快捷键说明.xlsx
@@ -9,12 +9,25 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="228">
   <si>
     <r>
       <rPr>
@@ -470,7 +483,20 @@
     <t>ctrl+shift+enter</t>
   </si>
   <si>
-    <t>完成当行代码，如括号、分号可自动补全，补全后再次敲击，可新起一行</t>
+    <t>完成当行代码，如括号、分号可自动补全，补全后再次敲击，可跳下一行（如是空行）（不同于shift+enter新起一行)
+Choose lookup item and invoke complete statement</t>
+  </si>
+  <si>
+    <t>ctrl+shift+j</t>
+  </si>
+  <si>
+    <t>Join lines, 将两行合成一行</t>
+  </si>
+  <si>
+    <t>ctrl+enter</t>
+  </si>
+  <si>
+    <t>split line，将一行拆分成两行</t>
   </si>
   <si>
     <t>ctrl+alt+t</t>
@@ -519,6 +545,18 @@
   </si>
   <si>
     <t>将该行代码下移</t>
+  </si>
+  <si>
+    <t>alt+shift+,</t>
+  </si>
+  <si>
+    <t>缩小所有编辑器的字体大小</t>
+  </si>
+  <si>
+    <t>alt+shift+.</t>
+  </si>
+  <si>
+    <t>增大所有编辑器的字体大小</t>
   </si>
   <si>
     <t>ctrl+shift+↑</t>
@@ -758,7 +796,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -1774,12 +1812,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A112" sqref="A112"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -2290,7 +2328,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" ht="27" spans="1:2">
+    <row r="64" ht="67.5" spans="1:2">
       <c r="A64" s="8" t="s">
         <v>124</v>
       </c>
@@ -2298,7 +2336,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" ht="27" spans="1:2">
+    <row r="65" spans="1:2">
       <c r="A65" s="8" t="s">
         <v>126</v>
       </c>
@@ -2307,26 +2345,26 @@
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" t="s">
+      <c r="A66" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="5" t="s">
+    <row r="67" ht="27" spans="1:2">
+      <c r="A67" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="9" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="5" t="s">
+      <c r="A68" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="1" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2362,7 +2400,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" ht="27" spans="1:2">
+    <row r="73" spans="1:2">
       <c r="A73" s="5" t="s">
         <v>142</v>
       </c>
@@ -2378,7 +2416,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" ht="27" spans="1:2">
+    <row r="75" spans="1:2">
       <c r="A75" s="5" t="s">
         <v>146</v>
       </c>
@@ -2387,18 +2425,18 @@
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" t="s">
+      <c r="A76" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
+    <row r="77" ht="27" spans="1:2">
+      <c r="A77" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="6" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2410,7 +2448,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" ht="27" spans="1:2">
       <c r="A79" s="5" t="s">
         <v>154</v>
       </c>
@@ -2419,34 +2457,34 @@
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="8" t="s">
+      <c r="A80" t="s">
         <v>156</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="81" ht="27" spans="1:2">
-      <c r="A81" s="8" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
         <v>158</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="83" ht="27" spans="1:2">
-      <c r="A83" s="8" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="6" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2458,7 +2496,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" ht="27" spans="1:2">
       <c r="A85" s="8" t="s">
         <v>166</v>
       </c>
@@ -2466,7 +2504,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" ht="27" spans="1:2">
+    <row r="86" spans="1:2">
       <c r="A86" s="8" t="s">
         <v>168</v>
       </c>
@@ -2474,7 +2512,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" ht="27" spans="1:2">
       <c r="A87" s="8" t="s">
         <v>170</v>
       </c>
@@ -2498,7 +2536,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" ht="27" spans="1:2">
       <c r="A90" s="8" t="s">
         <v>176</v>
       </c>
@@ -2507,78 +2545,78 @@
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" t="s">
+      <c r="A91" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" t="s">
+      <c r="A92" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="9" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" t="s">
+      <c r="A93" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="9" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" t="s">
+      <c r="A94" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="9" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="5" t="s">
+      <c r="A95" t="s">
         <v>186</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="5" t="s">
+      <c r="A96" t="s">
         <v>188</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="5" t="s">
+      <c r="A97" t="s">
         <v>190</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="98" ht="27" spans="1:2">
-      <c r="A98" s="8" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>192</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="1" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="8" t="s">
+      <c r="A99" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="100" ht="40.5" spans="1:2">
+    <row r="100" spans="1:2">
       <c r="A100" s="5" t="s">
         <v>196</v>
       </c>
@@ -2594,23 +2632,23 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="5" t="s">
+    <row r="102" ht="27" spans="1:2">
+      <c r="A102" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="9" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" ht="40.5" spans="1:2">
       <c r="A104" s="5" t="s">
         <v>204</v>
       </c>
@@ -2619,18 +2657,18 @@
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" t="s">
+      <c r="A105" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="106" ht="27" spans="1:2">
-      <c r="A106" s="8" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B106" s="6" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2638,31 +2676,31 @@
       <c r="A107" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="6" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="11" t="s">
+      <c r="A108" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="6" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="8" t="s">
+      <c r="A109" t="s">
         <v>214</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="110" ht="27" spans="1:2">
-      <c r="A110" t="s">
+      <c r="A110" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="9" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2672,6 +2710,38 @@
       </c>
       <c r="B111" s="5" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="114" ht="27" spans="1:2">
+      <c r="A114" t="s">
+        <v>224</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>